<commit_message>
Move ts definition away from SysSettings.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
+++ b/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698CA910-FFB2-4AC6-BE0F-8211BE0C5158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EEBEBB-8212-4149-8336-90BC2DB6B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
-    <sheet name="TimeSlices" sheetId="1" r:id="rId2"/>
-    <sheet name="RSDSOL" sheetId="2" r:id="rId3"/>
-    <sheet name="RSD_SH" sheetId="3" r:id="rId4"/>
-    <sheet name="RSD_RTFT" sheetId="4" r:id="rId5"/>
-    <sheet name="RSD_OE_DEM" sheetId="5" r:id="rId6"/>
-    <sheet name="PWR_AF" sheetId="6" r:id="rId7"/>
-    <sheet name="TRA_DEM" sheetId="7" r:id="rId8"/>
-    <sheet name="SRV_CS_DEM" sheetId="8" r:id="rId9"/>
-    <sheet name="SRV_PU_DEM" sheetId="9" r:id="rId10"/>
-    <sheet name="DCs" sheetId="10" r:id="rId11"/>
-    <sheet name="SRVSOL" sheetId="11" r:id="rId12"/>
+    <sheet name="TS_Definition" sheetId="13" r:id="rId2"/>
+    <sheet name="TimeSlices" sheetId="1" r:id="rId3"/>
+    <sheet name="RSDSOL" sheetId="2" r:id="rId4"/>
+    <sheet name="RSD_SH" sheetId="3" r:id="rId5"/>
+    <sheet name="RSD_RTFT" sheetId="4" r:id="rId6"/>
+    <sheet name="RSD_OE_DEM" sheetId="5" r:id="rId7"/>
+    <sheet name="PWR_AF" sheetId="6" r:id="rId8"/>
+    <sheet name="TRA_DEM" sheetId="7" r:id="rId9"/>
+    <sheet name="SRV_CS_DEM" sheetId="8" r:id="rId10"/>
+    <sheet name="SRV_PU_DEM" sheetId="9" r:id="rId11"/>
+    <sheet name="DCs" sheetId="10" r:id="rId12"/>
+    <sheet name="SRVSOL" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -92,12 +93,24 @@
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -343,6 +356,33 @@
   </si>
   <si>
     <t>Specify time slice data according to the time slice model variant</t>
+  </si>
+  <si>
+    <t>~TimeSlices</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>DayNite</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Hour</t>
   </si>
 </sst>
 </file>
@@ -352,7 +392,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -436,8 +476,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,13 +525,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -478,7 +564,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -535,6 +621,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -864,158 +955,217 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD8BDEB2-4A1A-4E46-B657-26B8126C13BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="571500"/>
+          <a:ext cx="3047999" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>~TimeSlices</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> is used to define</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>the time-slices resolution for the model, by declaring the elements of each time-slice: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SEASON</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WEEKLY </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DAYNITE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="timeslices" displayName="timeslices" ref="B2:AE3" totalsRowShown="0">
-  <autoFilter ref="B2:AE3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IE"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="National"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IE-CW"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="IE-D"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IE-KE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="IE-KK"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IE-LS"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IE-LD"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IE-LH"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IE-MH"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="IE-OY"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IE-WH"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IE-WX"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IE-WW"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IE-CE"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IE-CO"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="IE-KY"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IE-LK"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="IE-TA"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IE-WD"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IE-G"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IE-LM"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="IE-MO"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="IE-RN"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="IE-SO"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IE-CN"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IE-DL"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IE-MN"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B92864FE-A379-487D-9F3F-B9D210D4D9B4}" name="weekly_info" displayName="weekly_info" ref="O4:P11" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Day"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="dcs" displayName="dcs" ref="B2:I5" totalsRowShown="0">
-  <autoFilter ref="B2:I5" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Cset_CN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Pset_PN"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="srvsol" displayName="srvsol" ref="B2:I3" totalsRowShown="0">
-  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Pset_PN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Pset_CI"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:I3" totalsRowShown="0">
-  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Pset_PN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Pset_CI"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowShown="0">
-  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H3" totalsRowShown="0">
-  <autoFilter ref="B2:H3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
-    <tableColumn id="7" xr3:uid="{DA5FA9F4-D4B7-44E0-A803-2D2586DBF9CB}" name="LimType"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:G3" totalsRowShown="0">
-  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cset_CN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="pwr_af" displayName="pwr_af" ref="B2:G7" totalsRowShown="0">
-  <autoFilter ref="B2:G7" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Pset_PN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tra_dem" displayName="tra_dem" ref="B2:AG3" totalsRowShown="0">
   <autoFilter ref="B2:AG3" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="32">
@@ -1056,7 +1206,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="srv_cs_dem" displayName="srv_cs_dem" ref="B2:G3" totalsRowShown="0">
   <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="6">
@@ -1071,7 +1221,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="srv_pu_dem" displayName="srv_pu_dem" ref="B2:G3" totalsRowShown="0">
   <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="6">
@@ -1081,6 +1231,177 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Cset_CN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="IE"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="dcs" displayName="dcs" ref="B2:I5" totalsRowShown="0">
+  <autoFilter ref="B2:I5" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Cset_CN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Pset_PN"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="srvsol" displayName="srvsol" ref="B2:I3" totalsRowShown="0">
+  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Pset_PN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Pset_CI"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{8BAB9A19-16B1-439F-8D3B-1C87DDADB8BB}" name="season_info" displayName="season_info" ref="L4:M16" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Month"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Season"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{635E1DC4-6E84-4D32-AA40-E00034D55B90}" name="daynite_info" displayName="daynite_info" ref="R4:S28" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hour"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="timeslices" displayName="timeslices" ref="B2:AE3" totalsRowShown="0">
+  <autoFilter ref="B2:AE3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="30">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="National"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IE-CW"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="IE-D"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IE-KE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IE-MH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="IE-OY"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IE-WH"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IE-WX"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IE-WW"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IE-CE"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IE-CO"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="IE-KY"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IE-LK"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="IE-TA"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IE-WD"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IE-G"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IE-LM"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="IE-MO"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="IE-RN"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="IE-SO"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IE-CN"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IE-DL"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IE-MN"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:I3" totalsRowShown="0">
+  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Pset_PN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Pset_CI"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowShown="0">
+  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H3" totalsRowShown="0">
+  <autoFilter ref="B2:H3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
+    <tableColumn id="7" xr3:uid="{DA5FA9F4-D4B7-44E0-A803-2D2586DBF9CB}" name="LimType"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:G3" totalsRowShown="0">
+  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="pwr_af" displayName="pwr_af" ref="B2:G7" totalsRowShown="0">
+  <autoFilter ref="B2:G7" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1368,7 +1689,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
@@ -4216,6 +4537,69 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="B1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="B1:G3"/>
@@ -4278,7 +4662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:I5"/>
@@ -4393,7 +4777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="B1:I3"/>
@@ -4471,6 +4855,394 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E87912A-05C7-48D9-8B04-811783F0B11F}">
+  <dimension ref="B3:S28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" t="s">
+        <v>88</v>
+      </c>
+      <c r="R4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9" t="s">
+        <v>89</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
+      <c r="S12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13" t="s">
+        <v>89</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="S13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>89</v>
+      </c>
+      <c r="R14">
+        <v>9</v>
+      </c>
+      <c r="S14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15" t="s">
+        <v>89</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16">
+        <v>11</v>
+      </c>
+      <c r="S16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="R17">
+        <v>12</v>
+      </c>
+      <c r="S17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>13</v>
+      </c>
+      <c r="S18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>14</v>
+      </c>
+      <c r="S19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>15</v>
+      </c>
+      <c r="S20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>16</v>
+      </c>
+      <c r="S21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>17</v>
+      </c>
+      <c r="S22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>18</v>
+      </c>
+      <c r="S23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>19</v>
+      </c>
+      <c r="S24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>20</v>
+      </c>
+      <c r="S25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>21</v>
+      </c>
+      <c r="S26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>22</v>
+      </c>
+      <c r="S27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>23</v>
+      </c>
+      <c r="S28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AE3"/>
@@ -4679,7 +5451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:I3"/>
@@ -4756,7 +5528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:G3"/>
@@ -4819,7 +5591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H3"/>
@@ -4890,7 +5662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:G3"/>
@@ -4953,7 +5725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:G7"/>
@@ -5096,7 +5868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:AG3"/>
@@ -5313,67 +6085,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="B1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>2018</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Move TS definition to Scen_B_SYS_SubAnnual_Data.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
+++ b/SuppXLS/Scen_B_SYS_SubAnnual_Data.xlsx
@@ -1,35 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772630E7-62A9-43AA-925E-98B96D5768AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402F9C89-F88D-4257-9BED-136CAC25F9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
-    <sheet name="TimeSlices" sheetId="1" r:id="rId2"/>
-    <sheet name="RSDSOL" sheetId="2" r:id="rId3"/>
-    <sheet name="RSD_SH" sheetId="3" r:id="rId4"/>
-    <sheet name="RSD_RTFT" sheetId="4" r:id="rId5"/>
-    <sheet name="RSD_OE_DEM" sheetId="5" r:id="rId6"/>
-    <sheet name="PWR_AF" sheetId="6" r:id="rId7"/>
-    <sheet name="TRA_DEM" sheetId="7" r:id="rId8"/>
-    <sheet name="SRV_CS_DEM" sheetId="8" r:id="rId9"/>
-    <sheet name="SRV_PU_DEM" sheetId="9" r:id="rId10"/>
-    <sheet name="DCs" sheetId="10" r:id="rId11"/>
-    <sheet name="SRVSOL" sheetId="11" r:id="rId12"/>
+    <sheet name="TS_Definition" sheetId="13" r:id="rId2"/>
+    <sheet name="TimeSlices" sheetId="1" r:id="rId3"/>
+    <sheet name="RSDSOL" sheetId="2" r:id="rId4"/>
+    <sheet name="RSD_SH" sheetId="3" r:id="rId5"/>
+    <sheet name="RSD_RTFT" sheetId="4" r:id="rId6"/>
+    <sheet name="RSD_OE_DEM" sheetId="5" r:id="rId7"/>
+    <sheet name="PWR_AF" sheetId="6" r:id="rId8"/>
+    <sheet name="TRA_DEM" sheetId="7" r:id="rId9"/>
+    <sheet name="SRV_CS_DEM" sheetId="8" r:id="rId10"/>
+    <sheet name="SRV_PU_DEM" sheetId="9" r:id="rId11"/>
+    <sheet name="DCs" sheetId="10" r:id="rId12"/>
+    <sheet name="SRVSOL" sheetId="11" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">2</definedName>
@@ -51,10 +53,15 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
@@ -92,7 +99,9 @@
     <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
     <definedName name="RiskUseFixedSeed" hidden="1">TRUE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
+    <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -100,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="140">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -464,6 +473,63 @@
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
   </si>
+  <si>
+    <t>~TimeSlices</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>DayNite</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Wi</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Sp</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Au</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
 </sst>
 </file>
 
@@ -472,7 +538,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -556,8 +622,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,13 +671,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -598,7 +710,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -607,9 +719,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -637,9 +746,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -655,6 +761,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -984,11 +1101,212 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E53258A9-5C47-4713-B092-3E59E5324E40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="571500"/>
+          <a:ext cx="3047999" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>~TimeSlices</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> is used to define</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>the time-slices resolution for the model, by declaring the elements of each time-slice: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SEASON</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WEEKLY </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DAYNITE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover"/>
+      <sheetName val="TS_Definition"/>
       <sheetName val="TimeSlices"/>
       <sheetName val="RSDSOL"/>
       <sheetName val="RSD_SH"/>
@@ -1002,175 +1320,35 @@
       <sheetName val="SRVSOL"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="timeslices" displayName="timeslices" ref="B2:AE42" totalsRowShown="0">
-  <autoFilter ref="B2:AE42" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IE"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="National"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IE-CW"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="IE-D"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IE-KE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="IE-KK"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IE-LS"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IE-LD"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IE-LH"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IE-MH"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="IE-OY"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IE-WH"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IE-WX"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IE-WW"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IE-CE"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IE-CO"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="IE-KY"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IE-LK"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="IE-TA"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IE-WD"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IE-G"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IE-LM"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="IE-MO"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="IE-RN"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="IE-SO"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IE-CN"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IE-DL"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IE-MN"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00A0ED70-32B0-422F-A128-202FFFBDD989}" name="season_info19" displayName="season_info19" ref="L4:M16" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D2785796-31B0-4942-B2B3-FC23091CEF01}" name="Month"/>
+    <tableColumn id="2" xr3:uid="{A5E59FBE-8C76-43E0-A504-9175BB417965}" name="Season"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="dcs" displayName="dcs" ref="B2:I122" totalsRowShown="0">
-  <autoFilter ref="B2:I122" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Cset_CN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Pset_PN"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="srvsol" displayName="srvsol" ref="B2:I42" totalsRowShown="0">
-  <autoFilter ref="B2:I42" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Pset_PN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Pset_CI"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:I42" totalsRowShown="0">
-  <autoFilter ref="B2:I42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Other_Indexes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Pset_PN"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Pset_CI"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="IE"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G42" totalsRowShown="0">
-  <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H42" totalsRowShown="0">
-  <autoFilter ref="B2:H42" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
-    <tableColumn id="7" xr3:uid="{A089AEDA-8E96-495A-8524-E07DDD68F013}" name="LimType"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:G42" totalsRowShown="0">
-  <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cset_CN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="pwr_af" displayName="pwr_af" ref="B2:G202" totalsRowShown="0">
-  <autoFilter ref="B2:G202" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="TimeSlice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Pset_PN"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="IE"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="National"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tra_dem" displayName="tra_dem" ref="B2:AG42" totalsRowShown="0">
   <autoFilter ref="B2:AG42" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="32">
@@ -1211,7 +1389,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="srv_cs_dem" displayName="srv_cs_dem" ref="B2:G42" totalsRowShown="0">
   <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="6">
@@ -1226,7 +1404,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="srv_pu_dem" displayName="srv_pu_dem" ref="B2:G42" totalsRowShown="0">
   <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="6">
@@ -1236,6 +1414,177 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Cset_CN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="IE"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="dcs" displayName="dcs" ref="B2:I122" totalsRowShown="0">
+  <autoFilter ref="B2:I122" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Cset_CN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Pset_PN"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="srvsol" displayName="srvsol" ref="B2:I42" totalsRowShown="0">
+  <autoFilter ref="B2:I42" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Pset_PN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Pset_CI"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BD417E7D-061B-4101-B604-0FB95F82E942}" name="weekly_info20" displayName="weekly_info20" ref="O4:P11" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B647E062-A9E4-4FCD-A124-A965EDC97BFC}" name="Day"/>
+    <tableColumn id="2" xr3:uid="{2C6C4042-72B5-4245-9188-26A94F7DE2E4}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AE484DEB-DC4F-453D-859C-CB76072D019D}" name="daynite_info21" displayName="daynite_info21" ref="R4:S28" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B3AB0946-28C5-4E32-ABC2-54A46B2131D5}" name="Hour"/>
+    <tableColumn id="2" xr3:uid="{04684AF8-8A56-4F32-B901-103BAF315576}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="timeslices" displayName="timeslices" ref="B2:AE42" totalsRowShown="0">
+  <autoFilter ref="B2:AE42" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="30">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="National"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IE-CW"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="IE-D"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IE-KE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IE-MH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="IE-OY"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IE-WH"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IE-WX"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IE-WW"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IE-CE"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IE-CO"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="IE-KY"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IE-LK"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="IE-TA"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IE-WD"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IE-G"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IE-LM"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="IE-MO"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="IE-RN"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="IE-SO"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IE-CN"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IE-DL"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IE-MN"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:I42" totalsRowShown="0">
+  <autoFilter ref="B2:I42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Other_Indexes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Pset_PN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Pset_CI"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="IE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G42" totalsRowShown="0">
+  <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H42" totalsRowShown="0">
+  <autoFilter ref="B2:H42" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
+    <tableColumn id="7" xr3:uid="{A089AEDA-8E96-495A-8524-E07DDD68F013}" name="LimType"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:G42" totalsRowShown="0">
+  <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="pwr_af" displayName="pwr_af" ref="B2:G202" totalsRowShown="0">
+  <autoFilter ref="B2:G202" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1522,7 +1871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9E7995-53E7-4F58-976D-6AC1D3A1017B}">
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1959,20 +2308,20 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1989,10 +2338,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -2017,18 +2366,18 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -2045,22 +2394,22 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -2077,22 +2426,22 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -2109,22 +2458,22 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -2141,18 +2490,18 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -2169,14 +2518,14 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2201,10 +2550,10 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2229,10 +2578,10 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2257,14 +2606,14 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2289,10 +2638,10 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2317,10 +2666,10 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2345,14 +2694,14 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2377,16 +2726,16 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2409,16 +2758,16 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2441,12 +2790,12 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -4368,6 +4717,848 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B1:G42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3">
+        <v>1.661E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.661E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4">
+        <v>8.0400000000000003E-3</v>
+      </c>
+      <c r="G4">
+        <v>8.0400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5">
+        <v>2018</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5">
+        <v>3.32E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.32E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6">
+        <v>6.9100000000000003E-3</v>
+      </c>
+      <c r="G6">
+        <v>6.9100000000000003E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7">
+        <v>1.3169999999999999E-2</v>
+      </c>
+      <c r="G7">
+        <v>1.3169999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8">
+        <v>3.737E-2</v>
+      </c>
+      <c r="G8">
+        <v>3.737E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9">
+        <v>2018</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9">
+        <v>1.6719999999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.6719999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>2018</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10">
+        <v>7.1230000000000002E-2</v>
+      </c>
+      <c r="G10">
+        <v>7.1230000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11">
+        <v>2018</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11">
+        <v>1.538E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.538E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
+        <v>3.0269999999999998E-2</v>
+      </c>
+      <c r="G12">
+        <v>3.0269999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13">
+        <v>2018</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13">
+        <v>1.821E-2</v>
+      </c>
+      <c r="G13">
+        <v>1.821E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14">
+        <v>2018</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <v>8.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15">
+        <v>2018</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15">
+        <v>3.4979999999999997E-2</v>
+      </c>
+      <c r="G15">
+        <v>3.4979999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16">
+        <v>2018</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16">
+        <v>7.3200000000000001E-3</v>
+      </c>
+      <c r="G16">
+        <v>7.3200000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>2018</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17">
+        <v>1.4619999999999999E-2</v>
+      </c>
+      <c r="G17">
+        <v>1.4619999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18">
+        <v>2018</v>
+      </c>
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18">
+        <v>3.8190000000000002E-2</v>
+      </c>
+      <c r="G18">
+        <v>3.8190000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <v>2018</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19">
+        <v>1.6789999999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.6789999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20">
+        <v>2018</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20">
+        <v>7.1410000000000001E-2</v>
+      </c>
+      <c r="G20">
+        <v>7.1410000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21">
+        <v>2018</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21">
+        <v>1.5169999999999999E-2</v>
+      </c>
+      <c r="G21">
+        <v>1.5169999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22">
+        <v>2018</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="G22">
+        <v>3.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23">
+        <v>2018</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23">
+        <v>1.737E-2</v>
+      </c>
+      <c r="G23">
+        <v>1.737E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24">
+        <v>2018</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24">
+        <v>8.0499999999999999E-3</v>
+      </c>
+      <c r="G24">
+        <v>8.0499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25">
+        <v>2018</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25">
+        <v>3.2590000000000001E-2</v>
+      </c>
+      <c r="G25">
+        <v>3.2590000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>2018</v>
+      </c>
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26">
+        <v>6.45E-3</v>
+      </c>
+      <c r="G26">
+        <v>6.45E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27">
+        <v>1.2869999999999999E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.2869999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28">
+        <v>2018</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28">
+        <v>3.7909999999999999E-2</v>
+      </c>
+      <c r="G28">
+        <v>3.7909999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29">
+        <v>2018</v>
+      </c>
+      <c r="E29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29">
+        <v>1.669E-2</v>
+      </c>
+      <c r="G29">
+        <v>1.669E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30">
+        <v>2018</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30">
+        <v>6.8760000000000002E-2</v>
+      </c>
+      <c r="G30">
+        <v>6.8760000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31">
+        <v>2018</v>
+      </c>
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31">
+        <v>1.418E-2</v>
+      </c>
+      <c r="G31">
+        <v>1.418E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32">
+        <v>2018</v>
+      </c>
+      <c r="E32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32">
+        <v>2.903E-2</v>
+      </c>
+      <c r="G32">
+        <v>2.903E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33">
+        <v>2018</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33">
+        <v>1.7270000000000001E-2</v>
+      </c>
+      <c r="G33">
+        <v>1.7270000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34">
+        <v>2018</v>
+      </c>
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G34">
+        <v>7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35">
+        <v>2018</v>
+      </c>
+      <c r="E35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35">
+        <v>3.4909999999999997E-2</v>
+      </c>
+      <c r="G35">
+        <v>3.4909999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36">
+        <v>2018</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36">
+        <v>7.62E-3</v>
+      </c>
+      <c r="G36">
+        <v>7.62E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37">
+        <v>2018</v>
+      </c>
+      <c r="E37" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37">
+        <v>1.5049999999999999E-2</v>
+      </c>
+      <c r="G37">
+        <v>1.5049999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>2018</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="G38">
+        <v>3.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39">
+        <v>2018</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39">
+        <v>1.5630000000000002E-2</v>
+      </c>
+      <c r="G39">
+        <v>1.5630000000000002E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>2018</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40">
+        <v>7.0250000000000007E-2</v>
+      </c>
+      <c r="G40">
+        <v>7.0250000000000007E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>2018</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41">
+        <v>1.5469999999999999E-2</v>
+      </c>
+      <c r="G41">
+        <v>1.5469999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42">
+        <v>2018</v>
+      </c>
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42">
+        <v>3.124E-2</v>
+      </c>
+      <c r="G42">
+        <v>3.124E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:G42"/>
   <sheetViews>
@@ -5209,7 +6400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:I122"/>
   <sheetViews>
@@ -7897,7 +9088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:I42"/>
   <sheetViews>
@@ -8988,6 +10179,413 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A916DD6D-BEB6-4B16-A1CD-EEF48A0890F6}">
+  <dimension ref="B3:S28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>126</v>
+      </c>
+      <c r="P4" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>130</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>130</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>132</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>133</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>132</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>133</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9" t="s">
+        <v>133</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>132</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>132</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>134</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>131</v>
+      </c>
+      <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
+      <c r="S12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13" t="s">
+        <v>136</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="S13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R14">
+        <v>9</v>
+      </c>
+      <c r="S14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15" t="s">
+        <v>136</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16" t="s">
+        <v>130</v>
+      </c>
+      <c r="R16">
+        <v>11</v>
+      </c>
+      <c r="S16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="R17">
+        <v>12</v>
+      </c>
+      <c r="S17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>13</v>
+      </c>
+      <c r="S18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>14</v>
+      </c>
+      <c r="S19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>15</v>
+      </c>
+      <c r="S20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>16</v>
+      </c>
+      <c r="S21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>17</v>
+      </c>
+      <c r="S22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>18</v>
+      </c>
+      <c r="S23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>19</v>
+      </c>
+      <c r="S24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>20</v>
+      </c>
+      <c r="S25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>21</v>
+      </c>
+      <c r="S26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>22</v>
+      </c>
+      <c r="S27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>23</v>
+      </c>
+      <c r="S28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AE42"/>
   <sheetViews>
@@ -12783,7 +14381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I42"/>
   <sheetViews>
@@ -13873,7 +15471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G42"/>
   <sheetViews>
@@ -14715,7 +16313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H42"/>
   <sheetViews>
@@ -15685,7 +17283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:G42"/>
   <sheetViews>
@@ -16527,7 +18125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G202"/>
   <sheetViews>
@@ -20569,7 +22167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:AG42"/>
   <sheetViews>
@@ -24607,846 +26205,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B1:G42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3">
-        <v>2018</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3">
-        <v>1.661E-2</v>
-      </c>
-      <c r="G3">
-        <v>1.661E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4">
-        <v>2018</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4">
-        <v>8.0400000000000003E-3</v>
-      </c>
-      <c r="G4">
-        <v>8.0400000000000003E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5">
-        <v>2018</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5">
-        <v>3.32E-2</v>
-      </c>
-      <c r="G5">
-        <v>3.32E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6">
-        <v>2018</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6">
-        <v>6.9100000000000003E-3</v>
-      </c>
-      <c r="G6">
-        <v>6.9100000000000003E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7">
-        <v>2018</v>
-      </c>
-      <c r="E7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7">
-        <v>1.3169999999999999E-2</v>
-      </c>
-      <c r="G7">
-        <v>1.3169999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8">
-        <v>2018</v>
-      </c>
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8">
-        <v>3.737E-2</v>
-      </c>
-      <c r="G8">
-        <v>3.737E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9">
-        <v>2018</v>
-      </c>
-      <c r="E9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9">
-        <v>1.6719999999999999E-2</v>
-      </c>
-      <c r="G9">
-        <v>1.6719999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10">
-        <v>2018</v>
-      </c>
-      <c r="E10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10">
-        <v>7.1230000000000002E-2</v>
-      </c>
-      <c r="G10">
-        <v>7.1230000000000002E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11">
-        <v>2018</v>
-      </c>
-      <c r="E11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11">
-        <v>1.538E-2</v>
-      </c>
-      <c r="G11">
-        <v>1.538E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12">
-        <v>2018</v>
-      </c>
-      <c r="E12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12">
-        <v>3.0269999999999998E-2</v>
-      </c>
-      <c r="G12">
-        <v>3.0269999999999998E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13">
-        <v>2018</v>
-      </c>
-      <c r="E13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13">
-        <v>1.821E-2</v>
-      </c>
-      <c r="G13">
-        <v>1.821E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14">
-        <v>2018</v>
-      </c>
-      <c r="E14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14">
-        <v>8.3000000000000001E-3</v>
-      </c>
-      <c r="G14">
-        <v>8.3000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15">
-        <v>2018</v>
-      </c>
-      <c r="E15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15">
-        <v>3.4979999999999997E-2</v>
-      </c>
-      <c r="G15">
-        <v>3.4979999999999997E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16">
-        <v>2018</v>
-      </c>
-      <c r="E16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16">
-        <v>7.3200000000000001E-3</v>
-      </c>
-      <c r="G16">
-        <v>7.3200000000000001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17">
-        <v>2018</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17">
-        <v>1.4619999999999999E-2</v>
-      </c>
-      <c r="G17">
-        <v>1.4619999999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18">
-        <v>2018</v>
-      </c>
-      <c r="E18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18">
-        <v>3.8190000000000002E-2</v>
-      </c>
-      <c r="G18">
-        <v>3.8190000000000002E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19">
-        <v>2018</v>
-      </c>
-      <c r="E19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19">
-        <v>1.6789999999999999E-2</v>
-      </c>
-      <c r="G19">
-        <v>1.6789999999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20">
-        <v>2018</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20">
-        <v>7.1410000000000001E-2</v>
-      </c>
-      <c r="G20">
-        <v>7.1410000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21">
-        <v>2018</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21">
-        <v>1.5169999999999999E-2</v>
-      </c>
-      <c r="G21">
-        <v>1.5169999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22">
-        <v>2018</v>
-      </c>
-      <c r="E22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="G22">
-        <v>3.0599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23">
-        <v>2018</v>
-      </c>
-      <c r="E23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23">
-        <v>1.737E-2</v>
-      </c>
-      <c r="G23">
-        <v>1.737E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24">
-        <v>2018</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24">
-        <v>8.0499999999999999E-3</v>
-      </c>
-      <c r="G24">
-        <v>8.0499999999999999E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25">
-        <v>2018</v>
-      </c>
-      <c r="E25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25">
-        <v>3.2590000000000001E-2</v>
-      </c>
-      <c r="G25">
-        <v>3.2590000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26">
-        <v>2018</v>
-      </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26">
-        <v>6.45E-3</v>
-      </c>
-      <c r="G26">
-        <v>6.45E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27">
-        <v>2018</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27">
-        <v>1.2869999999999999E-2</v>
-      </c>
-      <c r="G27">
-        <v>1.2869999999999999E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28">
-        <v>2018</v>
-      </c>
-      <c r="E28" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28">
-        <v>3.7909999999999999E-2</v>
-      </c>
-      <c r="G28">
-        <v>3.7909999999999999E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29">
-        <v>2018</v>
-      </c>
-      <c r="E29" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29">
-        <v>1.669E-2</v>
-      </c>
-      <c r="G29">
-        <v>1.669E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30">
-        <v>2018</v>
-      </c>
-      <c r="E30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30">
-        <v>6.8760000000000002E-2</v>
-      </c>
-      <c r="G30">
-        <v>6.8760000000000002E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31">
-        <v>2018</v>
-      </c>
-      <c r="E31" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31">
-        <v>1.418E-2</v>
-      </c>
-      <c r="G31">
-        <v>1.418E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32">
-        <v>2018</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32">
-        <v>2.903E-2</v>
-      </c>
-      <c r="G32">
-        <v>2.903E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33">
-        <v>2018</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33">
-        <v>1.7270000000000001E-2</v>
-      </c>
-      <c r="G33">
-        <v>1.7270000000000001E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34">
-        <v>2018</v>
-      </c>
-      <c r="E34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="G34">
-        <v>7.9000000000000008E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35">
-        <v>2018</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35">
-        <v>3.4909999999999997E-2</v>
-      </c>
-      <c r="G35">
-        <v>3.4909999999999997E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36">
-        <v>2018</v>
-      </c>
-      <c r="E36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36">
-        <v>7.62E-3</v>
-      </c>
-      <c r="G36">
-        <v>7.62E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37">
-        <v>2018</v>
-      </c>
-      <c r="E37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37">
-        <v>1.5049999999999999E-2</v>
-      </c>
-      <c r="G37">
-        <v>1.5049999999999999E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38">
-        <v>2018</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38">
-        <v>3.6299999999999999E-2</v>
-      </c>
-      <c r="G38">
-        <v>3.6299999999999999E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39">
-        <v>2018</v>
-      </c>
-      <c r="E39" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39">
-        <v>1.5630000000000002E-2</v>
-      </c>
-      <c r="G39">
-        <v>1.5630000000000002E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40">
-        <v>2018</v>
-      </c>
-      <c r="E40" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40">
-        <v>7.0250000000000007E-2</v>
-      </c>
-      <c r="G40">
-        <v>7.0250000000000007E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41">
-        <v>2018</v>
-      </c>
-      <c r="E41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41">
-        <v>1.5469999999999999E-2</v>
-      </c>
-      <c r="G41">
-        <v>1.5469999999999999E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42">
-        <v>2018</v>
-      </c>
-      <c r="E42" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42">
-        <v>3.124E-2</v>
-      </c>
-      <c r="G42">
-        <v>3.124E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>